<commit_message>
New data and simulators up to 51
</commit_message>
<xml_diff>
--- a/Data/Old_Files/New_Demand_idea.xlsx
+++ b/Data/Old_Files/New_Demand_idea.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="125">
   <si>
     <t>NE</t>
   </si>
@@ -392,13 +392,16 @@
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t>Region:Month</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -427,8 +430,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -447,12 +456,57 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="51"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -479,12 +533,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="15" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1155,7 +1219,7 @@
   <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1284,6 +1348,15 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="H6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="3"/>
@@ -1300,6 +1373,13 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10">
+        <v>1.7701</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="3"/>
@@ -2834,6 +2914,12 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="You must enter a number between 0 and 4 (inclusive)" promptTitle="Pricing" prompt="Enter a number between 0 and 4 (inclusive)" sqref="J7">
+      <formula1>0</formula1>
+      <formula2>4</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>